<commit_message>
Added 'contains' logic to a specific KPI
</commit_message>
<xml_diff>
--- a/Projects/INBEVTRADMX/Data/inbevtradmx_template_4.xlsx
+++ b/Projects/INBEVTRADMX/Data/inbevtradmx_template_4.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="193">
   <si>
     <t xml:space="preserve">KPI Level 1 Name</t>
   </si>
@@ -242,7 +242,7 @@
     <t xml:space="preserve">SKU, Other, POS</t>
   </si>
   <si>
-    <t xml:space="preserve">2X58 1X33 MEGA CORONA LIGHT, Mega light, Premium Stella Michelob Cucapa_Sabor para conocedores, TendCardTriptico_Michelob, TendCardTriptico_Stella Artois, TendCardTriptico_Cucapa, 1X30MEGAC, 1X28MEGAC, Michelob POS Other, Stella Artois POS Other, Cucapa POS Other</t>
+    <t xml:space="preserve">2X58 1X33 MEGA CORONA LIGHT, Mega light, Premium Stella Michelob Cucapa_Sabor para conocedores, TendCardTriptico_Michelob, TendCardTriptico_Stella Artois, TendCardTriptico_Cucapa, 1X30MEGAC, 1X28MEGAC, Michelob POS Other, Stella Artois POS Other, Cucapa POS Other, Prop_poster_michelob_Occi, Michelob ultra_bote, Michelob ultra_front, Poster BD 6x70 - Michelob, 40x60_CL_Mega_1x30, Corona light_mega, 37_40x60_CLmega, CervezaCucapa_logo_negro, Michelob_Ultra_4_color, Stella_Artois_1_color, beerhouse_poster_40x60, 1X28MEGAC, TendCardTriptico_Stella Artois, TendCardTriptico_Michelob, TendCardTriptico_Cucapa, Promo 100 Premium_UL_CU_M_S, Promo 100 Premium_UL_CU_M_S_BOTE ULTRA, Michelob POS Other, Corona Light POS Other, Stella Artois POS Other, Cucapa POS Other, 1X20FAMP 2X22MEDIASC 2X58MEGAC 1X26MEGABL 1X28MEGACL_Tus favoritas al mejor precio, 2X50FAMC 2X22MEDIASC 2X58MEGAC 1X56MEGAE 1X29MEGACL_Tus favoritas al mejor precio, 2X50FAMP 2X22MEDIASC 2X58MEGAP 2X49MEGABL 1X28MEGACL_Tus favoritas al mejor precio, 2X58 1X33 MEGA CORONA LIGHT, 2X58MEGAC 1X29MEGACL 2X50FAMC 2X22MEDIASC_Disfrutalas al mejor precio, 2X58MEGAC 2X50FAMC 2X22MEDIASC 1X29MEGACL 1X25MEGABL 2X51MEGAE_Tus favoritas al mejor precio, 2X70FAMC 2X22MEDIASC 2X58MEGAC 1X26MEGAE 1X29MEGACL_Tus favorias al mejor precio, Mega light, Premium Stella Michelob Cucapa_Sabor para conocedores, 2X58MEGAP 1X29MEGACL 2X50FAMP 2X24MEDIASP_Disfrutalas al mejor precio, 2X58MEGAC 1X29MEGACL 1X25MEGABL 2X50FAMC 2X22MEDIASC_Tus favoritas al mejor precio, 2X40FAMP 2X24MEDIASP 2X58MEGAP 1X26MEGABL 1X28MEGACL_Tus favoritas al mejor precio, 2X50FAMP 2X24MEDIASP 2X58MEGAP 2X49MEGABL 1X28MEGACL_Tus favoritas al mejor precio, Hoegaarden POS Other, 2X58MEGAC 1X29MEGACL 2X50FAMC 2X22MEDIASC_Disfrutalas al mejor precio, MUNDIAL_C_V_ME_BL, MUNDIAL_V_C_ME_BL, MUNDIAL_BL_C_V_ME, MUNDAL_C_V_ME_BL_SURESTE6, MUNDIAL_C_V_ME_BL_V2, MUNDIAL_C_V_ME_BL_SURESTE, MUNDIAL_C_V_ME_BL_SURESTE_2, MUNDIAL_C_V_ME_SURESTE3, MUNDIAL_SURESTE, MUNDIAL_C_ME_BL_SURESTE_5, MUNDIAL_MANGAS, MUNDIAL_BL_C_ME, MUNDIAL_C_P_ME_BL, MUNDIAL_BL_C MEDIA_P_ME, Bocanegra POS Other, Corcholata Entrada, SABORPARACONOCEDORES_STE-MICH-CU_355ml_POSTER, SABORPARACONOCEDORES_STE-MICH-CU_POSTER, Termometro, SABORPARACONOCEDORES_STE-MICH-CU_ITSMO, 2X58_CL_MEGA_SEPT, 4X54_CL_BOTE_SEPT, 20x125_CL_CUARTO_SEPT, CL_MEGA-MEDIA-BOTE_SEPT, CL_MEGA-MEDIA-BOTE_SEPT_MR, OKTOBERFEST_MOD-CU-STE-MICH_MEDIA, OKTOBERFEST_CU-MOD-STE_MEDIA-BOTE_NORTE_OCT, OKTOBERFEST_CU-MOD-STE_MEDIA-BOTE_NORTE_OCT_MR, OKTOBERFEST_CU-MICH-STE-MOD_MEDIA-BOTE_NORTE2_OCT_MR, OKTOBERFEST_CU-MICH-STE-MOD_MEDIA-BOTE_OCT, OKTOBERFEST_CU-MICH-STE-MOD_MEDIA-BOTE_OCT_MR, OKTOBERFEST_CU-MOD-STE_MEDIA-BOTE_NORTE2_POP_MR, OKTOBERFEST_CU-MOD-MICH-STE-VCH_MEDIA-BOTE_OCT, OKTOBERFEST_CU-MOD-MICH-STE-VCH_MEDIA-BOTE_OCT_MR, OKTOBERFEST_MOD-CU-STE_TENDCARD 4X3_NORTE, OKTOBERFEST_MOD-CU-STE-MICH_TENDCARD 4X3, SABORPARACONOCEDORES_CU-STE-MICH_BOTE-MEDIA_CB, SABORPARACONOCEDORES_CU-STE-MICH_MEDIA-BOTE_NORTE, SABORPARACONOCEDORES, ESPECIALIDADES, STE, Mich</t>
   </si>
   <si>
     <t xml:space="preserve">Product Availability KPI: If in at least one of the scene types there is product type POS from selected SKUs, then pass.</t>
@@ -480,6 +480,9 @@
   </si>
   <si>
     <t xml:space="preserve">SC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2X58 1X33 MEGA CORONA LIGHT, Mega light, Premium Stella Michelob Cucapa_Sabor para conocedores, TendCardTriptico_Michelob, TendCardTriptico_Stella Artois, TendCardTriptico_Cucapa, 1X30MEGAC, 1X28MEGAC, Michelob POS Other, Stella Artois POS Other, Cucapa POS Other, Prop_poster_michelob_Occi, Michelob ultra_bote, Michelob ultra_front, Poster BD 6x70 - Michelob, 40x60_CL_Mega_1x30, Corona light_mega, 37_40x60_CLmega, CervezaCucapa_logo_negro, Michelob_Ultra_4_color, Stella_Artois_1_color, beerhouse_poster_40x60, 1X28MEGAC, TendCardTriptico_Stella Artois, TendCardTriptico_Michelob, TendCardTriptico_Cucapa, Promo 100 Premium_UL_CU_M_S, Promo 100 Premium_UL_CU_M_S_BOTE ULTRA, Michelob POS Other, Corona Light POS Other, Stella Artois POS Other, Cucapa POS Other, 1X20FAMP 2X22MEDIASC 2X58MEGAC 1X26MEGABL 1X28MEGACL_Tus favoritas al mejor precio, 2X50FAMC 2X22MEDIASC 2X58MEGAC 1X56MEGAE 1X29MEGACL_Tus favoritas al mejor precio, 2X50FAMP 2X22MEDIASC 2X58MEGAP 2X49MEGABL 1X28MEGACL_Tus favoritas al mejor precio, 2X58 1X33 MEGA CORONA LIGHT, 2X58MEGAC 1X29MEGACL 2X50FAMC 2X22MEDIASC_Disfrutalas al mejor precio, 2X58MEGAC 2X50FAMC 2X22MEDIASC 1X29MEGACL 1X25MEGABL 2X51MEGAE_Tus favoritas al mejor precio, 2X70FAMC 2X22MEDIASC 2X58MEGAC 1X26MEGAE 1X29MEGACL_Tus favorias al mejor precio, Mega light, Premium Stella Michelob Cucapa_Sabor para conocedores, 2X58MEGAP 1X29MEGACL 2X50FAMP 2X24MEDIASP_Disfrutalas al mejor precio, 2X58MEGAC 1X29MEGACL 1X25MEGABL 2X50FAMC 2X22MEDIASC_Tus favoritas al mejor precio, 2X40FAMP 2X24MEDIASP 2X58MEGAP 1X26MEGABL 1X28MEGACL_Tus favoritas al mejor precio, 2X50FAMP 2X24MEDIASP 2X58MEGAP 2X49MEGABL 1X28MEGACL_Tus favoritas al mejor precio, Hoegaarden POS Other, 2X58MEGAC 1X29MEGACL 2X50FAMC 2X22MEDIASC_Disfrutalas al mejor precio, MUNDIAL_C_V_ME_BL, MUNDIAL_V_C_ME_BL, MUNDIAL_BL_C_V_ME, MUNDAL_C_V_ME_BL_SURESTE6, MUNDIAL_C_V_ME_BL_V2, MUNDIAL_C_V_ME_BL_SURESTE, MUNDIAL_C_V_ME_BL_SURESTE_2, MUNDIAL_C_V_ME_SURESTE3, MUNDIAL_SURESTE, MUNDIAL_C_ME_BL_SURESTE_5, MUNDIAL_MANGAS, MUNDIAL_BL_C_ME, MUNDIAL_C_P_ME_BL, MUNDIAL_BL_C MEDIA_P_ME, Bocanegra POS Other, Corcholata Entrada, SABORPARACONOCEDORES_STE-MICH-CU_355ml_POSTER, SABORPARACONOCEDORES_STE-MICH-CU_POSTER, Termometro, SABORPARACONOCEDORES_STE-MICH-CU_ITSMO, 2X58_CL_MEGA_SEPT, 4X54_CL_BOTE_SEPT, 20x125_CL_CUARTO_SEPT, CL_MEGA-MEDIA-BOTE_SEPT, CL_MEGA-MEDIA-BOTE_SEPT_MR, OKTOBERFEST_MOD-CU-STE-MICH_MEDIA, OKTOBERFEST_CU-MOD-STE_MEDIA-BOTE_NORTE_OCT, OKTOBERFEST_CU-MOD-STE_MEDIA-BOTE_NORTE_OCT_MR, OKTOBERFEST_CU-MICH-STE-MOD_MEDIA-BOTE_NORTE2_OCT_MR, OKTOBERFEST_CU-MICH-STE-MOD_MEDIA-BOTE_OCT, OKTOBERFEST_CU-MICH-STE-MOD_MEDIA-BOTE_OCT_MR, OKTOBERFEST_CU-MOD-STE_MEDIA-BOTE_NORTE2_POP_MR, OKTOBERFEST_CU-MOD-MICH-STE-VCH_MEDIA-BOTE_OCT, OKTOBERFEST_CU-MOD-MICH-STE-VCH_MEDIA-BOTE_OCT_MR, OKTOBERFEST_MOD-CU-STE_TENDCARD 4X3_NORTE, OKTOBERFEST_MOD-CU-STE-MICH_TENDCARD 4X3, SABORPARACONOCEDORES_CU-STE-MICH_BOTE-MEDIA_CB, SABORPARACONOCEDORES_CU-STE-MICH_MEDIA-BOTE_NORTE,  SABORPARACONOCEDORES, ESPECIALIDADES, STE, Mich</t>
   </si>
   <si>
     <t xml:space="preserve">Set Botella Abierta Sin Cooler</t>
@@ -937,15 +940,19 @@
   </sheetPr>
   <dimension ref="A1:U65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R35" activeCellId="0" sqref="R35"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A30" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F43" activeCellId="0" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.3928571428571"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="41.3061224489796"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="55.8877551020408"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.1785714285714"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="39.8214285714286"/>
+    <col collapsed="false" hidden="false" max="19" min="7" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="53.8622448979592"/>
+    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1535,7 +1542,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
         <v>21</v>
       </c>
@@ -3368,7 +3375,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="8" t="s">
         <v>150</v>
       </c>
@@ -3384,7 +3391,7 @@
       </c>
       <c r="E43" s="8"/>
       <c r="F43" s="8" t="s">
-        <v>72</v>
+        <v>152</v>
       </c>
       <c r="G43" s="8"/>
       <c r="H43" s="8" t="s">
@@ -3428,7 +3435,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B44" s="8" t="s">
         <v>22</v>
@@ -3486,7 +3493,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B45" s="8" t="s">
         <v>78</v>
@@ -3546,7 +3553,7 @@
     </row>
     <row r="46" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B46" s="8" t="s">
         <v>81</v>
@@ -3606,10 +3613,10 @@
     </row>
     <row r="47" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C47" s="6" t="str">
         <f aca="false">B47</f>
@@ -3669,17 +3676,17 @@
         <v>90</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D48" s="6" t="s">
         <v>23</v>
       </c>
       <c r="E48" s="6"/>
       <c r="F48" s="6" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="G48" s="6" t="s">
         <v>24</v>
@@ -3711,10 +3718,10 @@
       </c>
       <c r="Q48" s="6"/>
       <c r="R48" s="16" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="S48" s="16" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="T48" s="10" t="s">
         <v>146</v>
@@ -3725,13 +3732,13 @@
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="19" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B49" s="19" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C49" s="19" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D49" s="19" t="s">
         <v>23</v>
@@ -3765,16 +3772,16 @@
         <v>94</v>
       </c>
       <c r="Q49" s="19" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="R49" s="19" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="S49" s="19" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="T49" s="21" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="U49" s="19" t="s">
         <v>32</v>
@@ -3782,13 +3789,13 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="19" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B50" s="19" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C50" s="19" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D50" s="19" t="s">
         <v>34</v>
@@ -3810,7 +3817,7 @@
         <v>24</v>
       </c>
       <c r="M50" s="19" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="N50" s="19" t="n">
         <v>50</v>
@@ -3822,16 +3829,16 @@
         <v>94</v>
       </c>
       <c r="Q50" s="19" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="R50" s="19" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="S50" s="19" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="T50" s="21" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="U50" s="19" t="s">
         <v>32</v>
@@ -3863,105 +3870,108 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+  </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="6" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="6" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="6" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C5" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="D5" s="0" t="s">
         <v>175</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="D11" s="0" t="s">
         <v>182</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
+        <v>186</v>
+      </c>
+      <c r="D13" s="0" t="s">
         <v>185</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -3987,6 +3997,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -4010,25 +4023,28 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -4054,10 +4070,13 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>